<commit_message>
final version for testing
</commit_message>
<xml_diff>
--- a/input/TEST.xlsx
+++ b/input/TEST.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pleger/Documents/Projects/ChinaSimulatioN_V2/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F417B411-5D53-6E4E-AF0A-14458C52A4C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86F8D742-95B7-0A4D-A11D-8B5FDEAEDAD4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{B078D86E-CB7D-D145-8E1E-BF1E3C336D06}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="33">
   <si>
     <t>Variables</t>
   </si>
@@ -108,9 +108,6 @@
   </si>
   <si>
     <t>FRIENDS</t>
-  </si>
-  <si>
-    <t>MARKETS</t>
   </si>
   <si>
     <t>LEVELS</t>
@@ -657,10 +654,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{907F1E5B-209D-BA4A-9A57-BB6890C684CF}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -670,10 +667,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B1">
-        <v>30</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -681,7 +678,7 @@
         <v>22</v>
       </c>
       <c r="B2">
-        <v>20</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -689,7 +686,7 @@
         <v>23</v>
       </c>
       <c r="B3" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -705,39 +702,39 @@
         <v>25</v>
       </c>
       <c r="B5">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B6">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B7">
-        <v>20</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B9">
-        <v>1.2</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -745,14 +742,6 @@
         <v>32</v>
       </c>
       <c r="B10">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="B11">
         <v>1</v>
       </c>
     </row>
@@ -1605,7 +1594,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B14" s="10">
         <v>5.62</v>

</xml_diff>